<commit_message>
Added 1st draft food Added 1st draft exposures
</commit_message>
<xml_diff>
--- a/input/Eurofood_PFOS_PFOA_072020.xlsx
+++ b/input/Eurofood_PFOS_PFOA_072020.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aeast\OneDrive - Environmental Protection Agency (EPA)\Profile\Desktop\LEM4\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/east_alexander_epa_gov/Documents/Profile/Desktop/LEM4/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{914C4540-8110-42DA-B4F1-11E39BE5B19D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{914C4540-8110-42DA-B4F1-11E39BE5B19D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{6C66A534-70C2-40BD-8238-3A29E5390123}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-4140" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Page" sheetId="4" r:id="rId1"/>
@@ -843,7 +843,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A5:R20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
@@ -3607,8 +3607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92C3EB05-7910-43F3-A751-A03A881F8E59}">
   <dimension ref="A1:H97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E69" sqref="E53:E69"/>
+    <sheetView topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="C101" sqref="C101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>